<commit_message>
Theme colors are now preserved
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Misc/CopyingWorksheets.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Misc/CopyingWorksheets.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <x:workbookPr codeName="ThisWorkbook"/>
   <x:bookViews>
     <x:workbookView firstSheet="0" activeTab="0"/>
   </x:bookViews>
@@ -997,7 +997,7 @@
   <x:sheetViews>
     <x:sheetView tabSelected="0" workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="9.85125" defaultRowHeight="15" customHeight="1"/>
+  <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
     <x:col min="1" max="1" width="3.710625" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="15.1090625" style="0" customWidth="1"/>
@@ -1189,7 +1189,7 @@
   <x:sheetViews>
     <x:sheetView tabSelected="0" workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="9.85125" defaultRowHeight="15" customHeight="1"/>
+  <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
     <x:col min="1" max="1" width="9.140625" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="7.1090625" style="0" customWidth="1"/>

</xml_diff>

<commit_message>
BREAKING CHANGE: table.Rows() now returns the entire table including headers and totals. table.Rows() should now be replaced with table.DataRange.Rows()
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Misc/CopyingWorksheets.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Misc/CopyingWorksheets.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <x:si>
     <x:t>FName</x:t>
   </x:si>
@@ -67,9 +67,6 @@
   </x:si>
   <x:si>
     <x:t>Sum Of Income</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CONCATENATE("Count: ", CountA(Headers[Table Headers]))</x:t>
   </x:si>
   <x:si>
     <x:t>Contacts</x:t>
@@ -1153,7 +1150,7 @@
   <x:sheetData>
     <x:row r="2" spans="1:6">
       <x:c r="B2" s="1" t="s">
-        <x:v>18</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C2" s="2" t="s"/>
       <x:c r="D2" s="2" t="s"/>

</xml_diff>

<commit_message>
Fixed issue when copying worksheets with headers and footers
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Misc/CopyingWorksheets.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Misc/CopyingWorksheets.xlsx
@@ -1120,7 +1120,14 @@
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
-  <x:headerFooter/>
+  <x:headerFooter differentOddEven="0" differentFirst="0" scaleWithDoc="1" alignWithMargins="1">
+    <x:oddHeader/>
+    <x:oddFooter/>
+    <x:evenHeader/>
+    <x:evenFooter/>
+    <x:firstHeader/>
+    <x:firstFooter/>
+  </x:headerFooter>
   <x:tableParts count="3">
     <x:tablePart r:id="rId13"/>
     <x:tablePart r:id="rId14"/>
@@ -1232,7 +1239,14 @@
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
-  <x:headerFooter/>
+  <x:headerFooter differentOddEven="0" differentFirst="0" scaleWithDoc="1" alignWithMargins="1">
+    <x:oddHeader/>
+    <x:oddFooter/>
+    <x:evenHeader/>
+    <x:evenFooter/>
+    <x:firstHeader/>
+    <x:firstFooter/>
+  </x:headerFooter>
   <x:tableParts count="0"/>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
Even more memory and performance improvements.
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Misc/CopyingWorksheets.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Misc/CopyingWorksheets.xlsx
@@ -356,10 +356,10 @@
     <x:xf numFmtId="1" fontId="0" fillId="0" borderId="9" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="1" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="15" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="1" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="15" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
@@ -454,11 +454,11 @@
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>

</xml_diff>